<commit_message>
update ph database and covariate locs
</commit_message>
<xml_diff>
--- a/data/ph_database.xlsx
+++ b/data/ph_database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbely/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbely/Desktop/GitHub things/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFF19EB1-D98C-2543-9B12-FBC8391FC1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E069E1-671B-2F45-A649-F55281661931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="8900" windowWidth="30660" windowHeight="13760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3740" yWindow="1660" windowWidth="30660" windowHeight="13760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="7" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="490">
   <si>
     <t>Author (us)</t>
   </si>
@@ -1668,9 +1668,6 @@
     <t>Heinze 2011 Changes</t>
   </si>
   <si>
-    <t>Yes, straw</t>
-  </si>
-  <si>
     <t>Composted farmyard manure</t>
   </si>
   <si>
@@ -1704,9 +1701,6 @@
     <t>pH(KCl)</t>
   </si>
   <si>
-    <t>Birkhofer 2008 oing-term</t>
-  </si>
-  <si>
     <t>ConMIN (conventional mineral)</t>
   </si>
   <si>
@@ -1753,6 +1747,27 @@
   </si>
   <si>
     <t>Marinari, S., Mancinelli, R., Campiglia, E., Grego, S. (2006). "Chemical and biological indicators of soil quality in organic and conventional farming systems in central Italy." Ecological indicators 6:701-711.</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes </t>
+  </si>
+  <si>
+    <t>Birkhofer 2008 long-term</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>conventinal</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>SKAL.nl</t>
   </si>
 </sst>
 </file>
@@ -2065,7 +2080,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -2148,6 +2163,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2157,10 +2174,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2721,13 +2734,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -3752,10 +3765,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A103DBEC-A1D7-474B-B93F-489E8658811F}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView zoomScale="139" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A18" zoomScale="139" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3780,15 +3793,15 @@
       <c r="C1" s="40"/>
       <c r="D1" s="40"/>
       <c r="E1" s="40"/>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="57" t="s">
         <v>217</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
@@ -4685,13 +4698,49 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="38" t="s">
-        <v>335</v>
-      </c>
-      <c r="B30" s="6"/>
+      <c r="A30" s="55" t="s">
+        <v>371</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>486</v>
+      </c>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="55" t="s">
+        <v>373</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>488</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="38" t="s">
+        <v>335</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4709,7 +4758,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A57" sqref="A57"/>
+      <selection pane="bottomRight" activeCell="S52" sqref="S52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4729,7 +4778,7 @@
     <col min="15" max="15" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.33203125" style="58" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
@@ -4791,7 +4840,7 @@
       <c r="Q1" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="R1" s="57" t="s">
+      <c r="R1" s="8" t="s">
         <v>108</v>
       </c>
       <c r="S1" s="8" t="s">
@@ -4833,7 +4882,7 @@
       <c r="AE1" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="AF1" s="60" t="s">
+      <c r="AF1" s="53" t="s">
         <v>428</v>
       </c>
     </row>
@@ -4874,7 +4923,7 @@
       <c r="O2" t="s">
         <v>346</v>
       </c>
-      <c r="R2" s="58">
+      <c r="R2">
         <v>1</v>
       </c>
       <c r="S2" t="s">
@@ -4939,8 +4988,11 @@
       <c r="O3" t="s">
         <v>346</v>
       </c>
-      <c r="R3" s="58">
+      <c r="R3">
         <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>487</v>
       </c>
       <c r="U3" t="s">
         <v>239</v>
@@ -5007,6 +5059,9 @@
       <c r="P4" t="s">
         <v>347</v>
       </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
       <c r="S4" t="s">
         <v>348</v>
       </c>
@@ -5069,6 +5124,12 @@
       <c r="N5">
         <v>251</v>
       </c>
+      <c r="O5" t="s">
+        <v>358</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
       <c r="S5" t="s">
         <v>348</v>
       </c>
@@ -5128,7 +5189,7 @@
       <c r="O6" t="s">
         <v>358</v>
       </c>
-      <c r="R6" s="58">
+      <c r="R6">
         <v>2</v>
       </c>
       <c r="S6" t="s">
@@ -5190,8 +5251,8 @@
       <c r="O7" t="s">
         <v>358</v>
       </c>
-      <c r="R7" s="58">
-        <v>1</v>
+      <c r="R7">
+        <v>2</v>
       </c>
       <c r="S7" t="s">
         <v>348</v>
@@ -5249,6 +5310,12 @@
       <c r="N8">
         <v>135</v>
       </c>
+      <c r="O8" t="s">
+        <v>358</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
       <c r="S8" t="s">
         <v>348</v>
       </c>
@@ -5305,6 +5372,12 @@
       <c r="N9">
         <v>354</v>
       </c>
+      <c r="O9" t="s">
+        <v>358</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
       <c r="S9" t="s">
         <v>348</v>
       </c>
@@ -5361,6 +5434,12 @@
       <c r="N10">
         <v>242</v>
       </c>
+      <c r="O10" t="s">
+        <v>358</v>
+      </c>
+      <c r="R10">
+        <v>2</v>
+      </c>
       <c r="S10" t="s">
         <v>348</v>
       </c>
@@ -5485,7 +5564,7 @@
       <c r="P12" t="s">
         <v>347</v>
       </c>
-      <c r="R12" s="58">
+      <c r="R12">
         <v>2</v>
       </c>
       <c r="S12" t="s">
@@ -5527,7 +5606,7 @@
         <v>40.299999999999997</v>
       </c>
       <c r="E13">
-        <v>4.26</v>
+        <v>-4.26</v>
       </c>
       <c r="F13">
         <v>5</v>
@@ -5550,7 +5629,7 @@
       <c r="O13" t="s">
         <v>366</v>
       </c>
-      <c r="R13" s="58">
+      <c r="R13">
         <v>2</v>
       </c>
       <c r="S13" t="s">
@@ -5592,7 +5671,7 @@
         <v>55.28</v>
       </c>
       <c r="E14">
-        <v>2.14</v>
+        <v>-2.14</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -5615,14 +5694,14 @@
       <c r="O14" t="s">
         <v>370</v>
       </c>
-      <c r="R14" s="58">
+      <c r="R14">
         <v>1</v>
       </c>
       <c r="S14" t="s">
         <v>267</v>
       </c>
       <c r="U14" t="s">
-        <v>371</v>
+        <v>486</v>
       </c>
       <c r="V14" t="s">
         <v>368</v>
@@ -5693,7 +5772,7 @@
         <v>377</v>
       </c>
       <c r="U15" t="s">
-        <v>373</v>
+        <v>488</v>
       </c>
       <c r="V15" t="s">
         <v>374</v>
@@ -5764,7 +5843,7 @@
         <v>377</v>
       </c>
       <c r="U16" t="s">
-        <v>371</v>
+        <v>486</v>
       </c>
       <c r="V16" t="s">
         <v>376</v>
@@ -5831,11 +5910,14 @@
       <c r="O17" t="s">
         <v>381</v>
       </c>
+      <c r="P17" t="s">
+        <v>483</v>
+      </c>
       <c r="S17" t="s">
         <v>348</v>
       </c>
       <c r="U17" t="s">
-        <v>371</v>
+        <v>486</v>
       </c>
       <c r="V17" t="s">
         <v>379</v>
@@ -5896,11 +5978,14 @@
       <c r="O18" t="s">
         <v>381</v>
       </c>
+      <c r="P18" t="s">
+        <v>483</v>
+      </c>
       <c r="S18" t="s">
         <v>348</v>
       </c>
       <c r="U18" t="s">
-        <v>371</v>
+        <v>486</v>
       </c>
       <c r="V18" t="s">
         <v>380</v>
@@ -5961,11 +6046,14 @@
       <c r="O19" t="s">
         <v>381</v>
       </c>
+      <c r="P19" t="s">
+        <v>483</v>
+      </c>
       <c r="S19" t="s">
         <v>348</v>
       </c>
       <c r="U19" t="s">
-        <v>371</v>
+        <v>486</v>
       </c>
       <c r="V19" t="s">
         <v>379</v>
@@ -6026,11 +6114,14 @@
       <c r="O20" t="s">
         <v>381</v>
       </c>
+      <c r="P20" t="s">
+        <v>483</v>
+      </c>
       <c r="S20" t="s">
         <v>348</v>
       </c>
       <c r="U20" t="s">
-        <v>371</v>
+        <v>486</v>
       </c>
       <c r="V20" t="s">
         <v>380</v>
@@ -6091,11 +6182,14 @@
       <c r="O21" t="s">
         <v>381</v>
       </c>
+      <c r="P21" t="s">
+        <v>483</v>
+      </c>
       <c r="S21" t="s">
         <v>348</v>
       </c>
       <c r="U21" t="s">
-        <v>371</v>
+        <v>486</v>
       </c>
       <c r="V21" t="s">
         <v>379</v>
@@ -6156,11 +6250,14 @@
       <c r="O22" t="s">
         <v>381</v>
       </c>
+      <c r="P22" t="s">
+        <v>483</v>
+      </c>
       <c r="S22" t="s">
         <v>348</v>
       </c>
       <c r="U22" t="s">
-        <v>371</v>
+        <v>486</v>
       </c>
       <c r="V22" t="s">
         <v>380</v>
@@ -6221,7 +6318,10 @@
       <c r="O23" t="s">
         <v>385</v>
       </c>
-      <c r="R23" s="58">
+      <c r="P23" t="s">
+        <v>347</v>
+      </c>
+      <c r="R23">
         <v>4</v>
       </c>
       <c r="S23" t="s">
@@ -6298,11 +6398,14 @@
       <c r="O24" t="s">
         <v>393</v>
       </c>
-      <c r="R24" s="58">
+      <c r="R24">
         <v>1</v>
       </c>
       <c r="S24" t="s">
         <v>377</v>
+      </c>
+      <c r="U24" t="s">
+        <v>386</v>
       </c>
       <c r="V24" t="s">
         <v>394</v>
@@ -6363,8 +6466,14 @@
       <c r="O25" t="s">
         <v>393</v>
       </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
       <c r="S25" t="s">
         <v>377</v>
+      </c>
+      <c r="U25" t="s">
+        <v>386</v>
       </c>
       <c r="V25" t="s">
         <v>395</v>
@@ -6425,6 +6534,9 @@
       <c r="O26" t="s">
         <v>393</v>
       </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
       <c r="S26" t="s">
         <v>377</v>
       </c>
@@ -6490,6 +6602,9 @@
       <c r="O27" t="s">
         <v>393</v>
       </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
       <c r="S27" t="s">
         <v>377</v>
       </c>
@@ -6555,8 +6670,14 @@
       <c r="O28" t="s">
         <v>393</v>
       </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
       <c r="S28" t="s">
         <v>377</v>
+      </c>
+      <c r="U28" t="s">
+        <v>280</v>
       </c>
       <c r="V28" t="s">
         <v>398</v>
@@ -6617,8 +6738,14 @@
       <c r="O29" t="s">
         <v>393</v>
       </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
       <c r="S29" t="s">
         <v>377</v>
+      </c>
+      <c r="U29" t="s">
+        <v>280</v>
       </c>
       <c r="V29" t="s">
         <v>399</v>
@@ -6679,6 +6806,9 @@
       <c r="O30" t="s">
         <v>393</v>
       </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
       <c r="S30" t="s">
         <v>377</v>
       </c>
@@ -6718,7 +6848,7 @@
         <v>37.799999999999997</v>
       </c>
       <c r="E31">
-        <v>5.16</v>
+        <v>-5.16</v>
       </c>
       <c r="F31">
         <v>5</v>
@@ -6744,7 +6874,7 @@
       <c r="O31" t="s">
         <v>407</v>
       </c>
-      <c r="R31" s="58">
+      <c r="R31">
         <v>2</v>
       </c>
       <c r="S31" t="s">
@@ -6789,7 +6919,7 @@
         <v>37.799999999999997</v>
       </c>
       <c r="E32">
-        <v>5.16</v>
+        <v>-5.16</v>
       </c>
       <c r="F32">
         <v>5</v>
@@ -6814,6 +6944,9 @@
       </c>
       <c r="O32" t="s">
         <v>406</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
       </c>
       <c r="S32" t="s">
         <v>377</v>
@@ -6877,7 +7010,7 @@
       <c r="O33" t="s">
         <v>410</v>
       </c>
-      <c r="R33" s="58">
+      <c r="R33">
         <v>4</v>
       </c>
       <c r="S33" t="s">
@@ -6936,7 +7069,7 @@
       <c r="O34" t="s">
         <v>410</v>
       </c>
-      <c r="R34" s="58">
+      <c r="R34">
         <v>4</v>
       </c>
       <c r="S34" t="s">
@@ -6946,7 +7079,7 @@
         <v>404</v>
       </c>
       <c r="U34" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="V34" t="s">
         <v>404</v>
@@ -6974,6 +7107,12 @@
       <c r="C35" t="s">
         <v>416</v>
       </c>
+      <c r="D35" t="s">
+        <v>489</v>
+      </c>
+      <c r="E35" t="s">
+        <v>489</v>
+      </c>
       <c r="G35">
         <v>2001</v>
       </c>
@@ -6991,6 +7130,9 @@
       </c>
       <c r="O35" t="s">
         <v>414</v>
+      </c>
+      <c r="U35" t="s">
+        <v>280</v>
       </c>
       <c r="V35" t="s">
         <v>413</v>
@@ -7024,6 +7166,12 @@
       <c r="C36" t="s">
         <v>416</v>
       </c>
+      <c r="D36" t="s">
+        <v>489</v>
+      </c>
+      <c r="E36" t="s">
+        <v>489</v>
+      </c>
       <c r="G36">
         <v>2001</v>
       </c>
@@ -7041,6 +7189,9 @@
       </c>
       <c r="O36" t="s">
         <v>414</v>
+      </c>
+      <c r="U36" t="s">
+        <v>280</v>
       </c>
       <c r="V36" t="s">
         <v>413</v>
@@ -7089,11 +7240,14 @@
       <c r="N37" t="s">
         <v>421</v>
       </c>
-      <c r="R37" s="59" t="s">
+      <c r="R37" s="54" t="s">
         <v>422</v>
       </c>
       <c r="T37" t="s">
         <v>423</v>
+      </c>
+      <c r="U37" t="s">
+        <v>280</v>
       </c>
       <c r="V37" t="s">
         <v>424</v>
@@ -7139,11 +7293,14 @@
       <c r="N38" t="s">
         <v>421</v>
       </c>
-      <c r="R38" s="59" t="s">
+      <c r="R38" s="54" t="s">
         <v>422</v>
       </c>
       <c r="T38" t="s">
         <v>423</v>
+      </c>
+      <c r="U38" t="s">
+        <v>280</v>
       </c>
       <c r="V38" t="s">
         <v>424</v>
@@ -7207,7 +7364,7 @@
       <c r="O39" t="s">
         <v>431</v>
       </c>
-      <c r="R39" s="58">
+      <c r="R39">
         <v>2</v>
       </c>
       <c r="S39" t="s">
@@ -7215,6 +7372,9 @@
       </c>
       <c r="T39" t="s">
         <v>432</v>
+      </c>
+      <c r="U39" t="s">
+        <v>280</v>
       </c>
       <c r="V39" t="s">
         <v>413</v>
@@ -7272,14 +7432,20 @@
       <c r="N40">
         <v>50</v>
       </c>
-      <c r="R40" s="58">
-        <v>1</v>
+      <c r="P40" t="s">
+        <v>347</v>
+      </c>
+      <c r="R40">
+        <v>4</v>
       </c>
       <c r="S40" t="s">
         <v>437</v>
       </c>
       <c r="T40" t="s">
         <v>446</v>
+      </c>
+      <c r="U40" t="s">
+        <v>280</v>
       </c>
       <c r="V40" t="s">
         <v>439</v>
@@ -7334,14 +7500,20 @@
       <c r="N41">
         <v>50</v>
       </c>
-      <c r="R41" s="58">
-        <v>1</v>
+      <c r="P41" t="s">
+        <v>347</v>
+      </c>
+      <c r="R41">
+        <v>4</v>
       </c>
       <c r="S41" t="s">
         <v>437</v>
       </c>
       <c r="T41" t="s">
         <v>447</v>
+      </c>
+      <c r="U41" t="s">
+        <v>280</v>
       </c>
       <c r="V41" t="s">
         <v>440</v>
@@ -7396,14 +7568,20 @@
       <c r="N42">
         <v>50</v>
       </c>
-      <c r="R42" s="58">
-        <v>1</v>
+      <c r="P42" t="s">
+        <v>347</v>
+      </c>
+      <c r="R42">
+        <v>4</v>
       </c>
       <c r="S42" t="s">
         <v>437</v>
       </c>
       <c r="T42" t="s">
         <v>448</v>
+      </c>
+      <c r="U42" t="s">
+        <v>280</v>
       </c>
       <c r="V42" t="s">
         <v>441</v>
@@ -7458,14 +7636,20 @@
       <c r="N43">
         <v>50</v>
       </c>
-      <c r="R43" s="58">
-        <v>1</v>
+      <c r="P43" t="s">
+        <v>347</v>
+      </c>
+      <c r="R43">
+        <v>4</v>
       </c>
       <c r="S43" t="s">
         <v>437</v>
       </c>
       <c r="T43" t="s">
         <v>449</v>
+      </c>
+      <c r="U43" t="s">
+        <v>280</v>
       </c>
       <c r="V43" t="s">
         <v>442</v>
@@ -7520,14 +7704,20 @@
       <c r="N44">
         <v>50</v>
       </c>
-      <c r="R44" s="58">
-        <v>1</v>
+      <c r="P44" t="s">
+        <v>347</v>
+      </c>
+      <c r="R44">
+        <v>4</v>
       </c>
       <c r="S44" t="s">
         <v>437</v>
       </c>
       <c r="T44" t="s">
         <v>450</v>
+      </c>
+      <c r="U44" t="s">
+        <v>280</v>
       </c>
       <c r="V44" t="s">
         <v>443</v>
@@ -7582,14 +7772,20 @@
       <c r="N45">
         <v>50</v>
       </c>
-      <c r="R45" s="58">
-        <v>1</v>
+      <c r="P45" t="s">
+        <v>347</v>
+      </c>
+      <c r="R45">
+        <v>4</v>
       </c>
       <c r="S45" t="s">
         <v>437</v>
       </c>
       <c r="T45" t="s">
         <v>451</v>
+      </c>
+      <c r="U45" t="s">
+        <v>280</v>
       </c>
       <c r="V45" t="s">
         <v>444</v>
@@ -7644,14 +7840,20 @@
       <c r="N46">
         <v>50</v>
       </c>
-      <c r="R46" s="58">
-        <v>1</v>
+      <c r="P46" t="s">
+        <v>347</v>
+      </c>
+      <c r="R46">
+        <v>4</v>
       </c>
       <c r="S46" t="s">
         <v>437</v>
       </c>
       <c r="T46" t="s">
         <v>452</v>
+      </c>
+      <c r="U46" t="s">
+        <v>280</v>
       </c>
       <c r="V46" t="s">
         <v>445</v>
@@ -7704,7 +7906,10 @@
         <v>50</v>
       </c>
       <c r="P47" t="s">
-        <v>456</v>
+        <v>484</v>
+      </c>
+      <c r="R47">
+        <v>4</v>
       </c>
       <c r="S47" t="s">
         <v>349</v>
@@ -7713,10 +7918,10 @@
         <v>280</v>
       </c>
       <c r="V47" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="W47" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="Z47">
         <v>4</v>
@@ -7763,7 +7968,10 @@
         <v>50</v>
       </c>
       <c r="P48" t="s">
-        <v>456</v>
+        <v>484</v>
+      </c>
+      <c r="R48">
+        <v>4</v>
       </c>
       <c r="S48" t="s">
         <v>349</v>
@@ -7772,10 +7980,10 @@
         <v>280</v>
       </c>
       <c r="V48" t="s">
+        <v>457</v>
+      </c>
+      <c r="W48" t="s">
         <v>458</v>
-      </c>
-      <c r="W48" t="s">
-        <v>459</v>
       </c>
       <c r="Z48">
         <v>4</v>
@@ -7798,7 +8006,7 @@
         <v>20</v>
       </c>
       <c r="C49" t="s">
-        <v>468</v>
+        <v>485</v>
       </c>
       <c r="D49">
         <v>47.5</v>
@@ -7831,16 +8039,16 @@
         <v>280</v>
       </c>
       <c r="V49" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="W49" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="Z49">
         <v>4</v>
       </c>
       <c r="AA49" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AB49">
         <v>5.8</v>
@@ -7857,7 +8065,7 @@
         <v>20</v>
       </c>
       <c r="C50" t="s">
-        <v>468</v>
+        <v>485</v>
       </c>
       <c r="D50">
         <v>47.5</v>
@@ -7883,24 +8091,23 @@
       <c r="N50">
         <v>150</v>
       </c>
-      <c r="R50"/>
-      <c r="S50" s="58" t="s">
+      <c r="S50" t="s">
         <v>349</v>
       </c>
       <c r="U50" t="s">
         <v>280</v>
       </c>
       <c r="V50" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="W50" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="Z50">
         <v>4</v>
       </c>
       <c r="AA50" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AB50">
         <v>5.5</v>
@@ -7917,7 +8124,7 @@
         <v>20</v>
       </c>
       <c r="C51" t="s">
-        <v>468</v>
+        <v>485</v>
       </c>
       <c r="D51">
         <v>47.5</v>
@@ -7950,16 +8157,16 @@
         <v>280</v>
       </c>
       <c r="V51" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="W51" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="Z51">
         <v>4</v>
       </c>
       <c r="AA51" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AB51">
         <v>5.2</v>
@@ -7976,7 +8183,7 @@
         <v>21</v>
       </c>
       <c r="C52" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D52">
         <v>47.5</v>
@@ -8003,28 +8210,28 @@
         <v>150</v>
       </c>
       <c r="O52" t="s">
+        <v>470</v>
+      </c>
+      <c r="R52" t="s">
+        <v>469</v>
+      </c>
+      <c r="S52" t="s">
+        <v>471</v>
+      </c>
+      <c r="T52" t="s">
         <v>472</v>
-      </c>
-      <c r="R52" s="58" t="s">
-        <v>471</v>
-      </c>
-      <c r="S52" t="s">
-        <v>473</v>
-      </c>
-      <c r="T52" t="s">
-        <v>474</v>
       </c>
       <c r="U52" t="s">
         <v>280</v>
       </c>
       <c r="W52" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="Z52">
         <v>4</v>
       </c>
       <c r="AA52" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="AB52">
         <v>6.4</v>
@@ -8041,7 +8248,7 @@
         <v>21</v>
       </c>
       <c r="C53" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D53">
         <v>47.5</v>
@@ -8068,25 +8275,25 @@
         <v>150</v>
       </c>
       <c r="O53" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="S53" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="T53" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="U53" t="s">
         <v>280</v>
       </c>
       <c r="W53" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="Z53">
         <v>4</v>
       </c>
       <c r="AA53" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="AB53">
         <v>6.5</v>
@@ -8103,7 +8310,7 @@
         <v>21</v>
       </c>
       <c r="C54" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D54">
         <v>47.5</v>
@@ -8130,25 +8337,25 @@
         <v>150</v>
       </c>
       <c r="O54" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="S54" t="s">
+        <v>471</v>
+      </c>
+      <c r="T54" t="s">
         <v>473</v>
-      </c>
-      <c r="T54" t="s">
-        <v>475</v>
       </c>
       <c r="U54" t="s">
         <v>280</v>
       </c>
       <c r="W54" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="Z54">
         <v>4</v>
       </c>
       <c r="AA54" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="AB54">
         <v>6.2</v>
@@ -8165,7 +8372,7 @@
         <v>21</v>
       </c>
       <c r="C55" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D55">
         <v>47.5</v>
@@ -8192,25 +8399,25 @@
         <v>150</v>
       </c>
       <c r="O55" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="S55" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="T55" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="U55" t="s">
         <v>280</v>
       </c>
       <c r="W55" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="Z55">
         <v>4</v>
       </c>
       <c r="AA55" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="AB55">
         <v>6.2</v>
@@ -8227,7 +8434,7 @@
         <v>21</v>
       </c>
       <c r="C56" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D56">
         <v>47.5</v>
@@ -8254,22 +8461,25 @@
         <v>150</v>
       </c>
       <c r="O56" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="S56" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="T56" t="s">
-        <v>481</v>
+        <v>479</v>
+      </c>
+      <c r="U56" t="s">
+        <v>280</v>
       </c>
       <c r="W56" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="Z56">
         <v>4</v>
       </c>
       <c r="AA56" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="AB56">
         <v>6</v>
@@ -8286,7 +8496,7 @@
         <v>21</v>
       </c>
       <c r="C57" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D57">
         <v>47.5</v>
@@ -8313,22 +8523,25 @@
         <v>150</v>
       </c>
       <c r="O57" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="S57" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="T57" t="s">
-        <v>482</v>
+        <v>480</v>
+      </c>
+      <c r="U57" t="s">
+        <v>280</v>
       </c>
       <c r="W57" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="Z57">
         <v>4</v>
       </c>
       <c r="AA57" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="AB57">
         <v>6.1</v>
@@ -8345,7 +8558,7 @@
         <v>21</v>
       </c>
       <c r="C58" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D58">
         <v>47.5</v>
@@ -8372,22 +8585,22 @@
         <v>150</v>
       </c>
       <c r="O58" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="S58" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="U58" t="s">
         <v>386</v>
       </c>
       <c r="W58" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="Z58">
         <v>4</v>
       </c>
       <c r="AA58" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="AB58">
         <v>6</v>
@@ -8588,7 +8801,7 @@
         <v>430</v>
       </c>
       <c r="C16" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -8607,10 +8820,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C18" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -8618,10 +8831,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
+        <v>460</v>
+      </c>
+      <c r="C19" t="s">
         <v>461</v>
-      </c>
-      <c r="C19" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -8629,10 +8842,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C20" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -8641,18 +8854,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <WPleader xmlns="5db17345-b4eb-4637-a02c-6c069878d2b2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5db17345-b4eb-4637-a02c-6c069878d2b2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b0e85a64-8fc1-4bad-a10c-f0bc3ffd3009" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -8661,7 +8862,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100805C233095455B4E8D77A60418F63AE2" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d8f27682910d1cad1581df4c3225fcbd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5db17345-b4eb-4637-a02c-6c069878d2b2" xmlns:ns3="b0e85a64-8fc1-4bad-a10c-f0bc3ffd3009" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="82f5adcd2403d076c54f7052aba3d40c" ns2:_="" ns3:_="">
     <xsd:import namespace="5db17345-b4eb-4637-a02c-6c069878d2b2"/>
@@ -8909,18 +9110,19 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B35628C1-6DED-4DF9-94F5-BE9AF8F77FE0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5db17345-b4eb-4637-a02c-6c069878d2b2"/>
-    <ds:schemaRef ds:uri="b0e85a64-8fc1-4bad-a10c-f0bc3ffd3009"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <WPleader xmlns="5db17345-b4eb-4637-a02c-6c069878d2b2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5db17345-b4eb-4637-a02c-6c069878d2b2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b0e85a64-8fc1-4bad-a10c-f0bc3ffd3009" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38497684-139F-4009-AAC9-C56DFE36120B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -8928,7 +9130,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89D612EE-02F0-4BD6-9117-3446EF205585}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8945,4 +9147,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B35628C1-6DED-4DF9-94F5-BE9AF8F77FE0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5db17345-b4eb-4637-a02c-6c069878d2b2"/>
+    <ds:schemaRef ds:uri="b0e85a64-8fc1-4bad-a10c-f0bc3ffd3009"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>